<commit_message>
Updates to code, figures, and manuscript
</commit_message>
<xml_diff>
--- a/Data/Derived/rf_performance_metrics.xlsx
+++ b/Data/Derived/rf_performance_metrics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis\Documents\GitHub\Collins_Pine\Data\Derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8FF74A0-4980-4313-81FB-906D4E836385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16C663D-B715-4CE3-9481-F8E7762573FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A70C1A4F-67E2-4FD5-82EE-839CF4CAC3BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,10 +435,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -449,10 +449,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -477,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -491,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -505,7 +505,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -519,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -547,10 +547,10 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -589,7 +589,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>0.06</v>

</xml_diff>